<commit_message>
DOC: Add v1.33.0 release notes
</commit_message>
<xml_diff>
--- a/gramex/apps/guide/auth/lookup.xlsx
+++ b/gramex/apps/guide/auth/lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\site\gramener.com\viz\async-gramex\gramex\apps\guide\auth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{10472AA3-3DEC-4250-A897-F4B8A7D45201}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CB46C64C-D336-41AE-9AA5-6508F2D1AC97}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="3480" xr2:uid="{A3983844-33D8-472B-8D33-EA42E9B2A6FF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>user</t>
   </si>
@@ -43,6 +43,30 @@
   </si>
   <si>
     <t>beta</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>superuser</t>
+  </si>
+  <si>
+    <t>tenure</t>
   </si>
 </sst>
 </file>
@@ -78,8 +102,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,39 +419,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7962F0-29C9-4C0A-BBE0-909ACB998AAA}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>103</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>